<commit_message>
Roundtrip redone; Results wording consistent with other tests.
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\mk-home\GitHub\bpmn-miwg-test-suite-fork\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="11640" tabRatio="631" firstSheet="1" activeTab="1"/>
   </bookViews>
@@ -20,7 +25,7 @@
     <author>Mélanie Gauthier</author>
   </authors>
   <commentList>
-    <comment ref="D25" authorId="0">
+    <comment ref="D25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F25" authorId="0">
+    <comment ref="F25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -68,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D45" authorId="0">
+    <comment ref="D45" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -92,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F45" authorId="0">
+    <comment ref="F45" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -116,7 +121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D59" authorId="0">
+    <comment ref="D59" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F59" authorId="0">
+    <comment ref="F59" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -174,7 +179,7 @@
     <author>matthias</author>
   </authors>
   <commentList>
-    <comment ref="K2" authorId="0">
+    <comment ref="K2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -198,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0">
+    <comment ref="I5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -223,7 +228,106 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0">
+    <comment ref="K5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>matthias:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+No Connections
+Events not aligned</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>matthias:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+No Connections
+Events not aligned</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>matthias:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+No Connections
+Events not aligned</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>matthias:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+There is a general Problem with importing the graphical representation.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -252,7 +356,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="87">
   <si>
     <t>Documentation</t>
   </si>
@@ -586,9 +690,6 @@
     <t>MID Innovator</t>
   </si>
   <si>
-    <t>Failed</t>
-  </si>
-  <si>
     <t>Import</t>
   </si>
   <si>
@@ -604,21 +705,21 @@
     <t>OK</t>
   </si>
   <si>
-    <t>Failed
-Implicitly</t>
-  </si>
-  <si>
     <t>Signavio Process Editor</t>
   </si>
   <si>
     <t>Issues</t>
+  </si>
+  <si>
+    <t>Issues
+(impl.)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -723,7 +824,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -1218,17 +1319,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1319,7 +1409,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1466,32 +1556,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1517,109 +1623,67 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1635,9 +1699,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1675,9 +1739,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1709,9 +1773,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1743,9 +1808,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1918,14 +1984,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
@@ -1934,8 +2000,8 @@
     <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:11" ht="125.25" customHeight="1" thickBot="1">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="125.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="5" t="s">
         <v>38</v>
       </c>
@@ -1967,17 +2033,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="2:11">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>41</v>
       </c>
@@ -1989,7 +2055,7 @@
       </c>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D18" s="10" t="s">
         <v>9</v>
       </c>
@@ -2000,7 +2066,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D19" s="10" t="s">
         <v>10</v>
       </c>
@@ -2011,7 +2077,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D20" s="10" t="s">
         <v>11</v>
       </c>
@@ -2022,7 +2088,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D21" s="10" t="s">
         <v>12</v>
       </c>
@@ -2031,7 +2097,7 @@
       </c>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D22" s="10" t="s">
         <v>46</v>
       </c>
@@ -2042,7 +2108,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D23" s="10" t="s">
         <v>18</v>
       </c>
@@ -2053,7 +2119,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D24" s="10" t="s">
         <v>47</v>
       </c>
@@ -2064,7 +2130,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D25" s="18" t="s">
         <v>49</v>
       </c>
@@ -2075,7 +2141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>42</v>
       </c>
@@ -2087,7 +2153,7 @@
       </c>
       <c r="F37" s="11"/>
     </row>
-    <row r="38" spans="2:6">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D38" s="10" t="s">
         <v>9</v>
       </c>
@@ -2098,7 +2164,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="2:6">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D39" s="10" t="s">
         <v>10</v>
       </c>
@@ -2109,7 +2175,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="2:6">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D40" s="10" t="s">
         <v>11</v>
       </c>
@@ -2120,7 +2186,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D41" s="10" t="s">
         <v>12</v>
       </c>
@@ -2129,7 +2195,7 @@
       </c>
       <c r="F41" s="11"/>
     </row>
-    <row r="42" spans="2:6">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D42" s="10" t="s">
         <v>46</v>
       </c>
@@ -2140,7 +2206,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="2:6">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D43" s="10" t="s">
         <v>18</v>
       </c>
@@ -2151,7 +2217,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="2:6">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D44" s="10" t="s">
         <v>47</v>
       </c>
@@ -2162,7 +2228,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="2:6">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D45" s="13" t="s">
         <v>49</v>
       </c>
@@ -2173,7 +2239,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="2:6">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D46" s="14" t="s">
         <v>1</v>
       </c>
@@ -2182,7 +2248,7 @@
       </c>
       <c r="F46" s="16"/>
     </row>
-    <row r="51" spans="2:6">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>43</v>
       </c>
@@ -2194,7 +2260,7 @@
       </c>
       <c r="F51" s="11"/>
     </row>
-    <row r="52" spans="2:6">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D52" s="10" t="s">
         <v>9</v>
       </c>
@@ -2205,7 +2271,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="2:6">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D53" s="10" t="s">
         <v>10</v>
       </c>
@@ -2216,7 +2282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="2:6">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D54" s="10" t="s">
         <v>11</v>
       </c>
@@ -2227,7 +2293,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="2:6">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D55" s="10" t="s">
         <v>12</v>
       </c>
@@ -2236,7 +2302,7 @@
       </c>
       <c r="F55" s="11"/>
     </row>
-    <row r="56" spans="2:6">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D56" s="10" t="s">
         <v>46</v>
       </c>
@@ -2247,7 +2313,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="2:6">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D57" s="10" t="s">
         <v>18</v>
       </c>
@@ -2258,7 +2324,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="2:6">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D58" s="10" t="s">
         <v>47</v>
       </c>
@@ -2269,7 +2335,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="2:6">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D59" s="13" t="s">
         <v>49</v>
       </c>
@@ -2280,7 +2346,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="2:6">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D60" s="17" t="s">
         <v>21</v>
       </c>
@@ -2291,7 +2357,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="2:6">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D61" s="15" t="s">
         <v>22</v>
       </c>
@@ -2302,12 +2368,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="2:2">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="2:2">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>45</v>
       </c>
@@ -2339,17 +2405,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" customWidth="1"/>
@@ -2360,19 +2426,19 @@
     <col min="8" max="8" width="54.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="46.5" thickBot="1">
-      <c r="A2" s="73" t="s">
+    <row r="2" spans="1:15" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="73" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="74"/>
-      <c r="E2" s="73" t="s">
+      <c r="D2" s="67"/>
+      <c r="E2" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="74"/>
+      <c r="F2" s="67"/>
       <c r="G2" s="24" t="s">
         <v>36</v>
       </c>
@@ -2380,26 +2446,26 @@
         <v>33</v>
       </c>
       <c r="I2" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="55" t="s">
+      <c r="K2" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="K2" s="55" t="s">
-        <v>82</v>
-      </c>
-      <c r="L2" s="77" t="s">
+      <c r="L2" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="M2" s="77" t="s">
+      <c r="N2" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="N2" s="77" t="s">
-        <v>82</v>
-      </c>
-      <c r="O2" s="75"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1">
+      <c r="O2" s="57"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="50"/>
       <c r="B3" s="51"/>
       <c r="C3" s="52"/>
@@ -2408,18 +2474,18 @@
       <c r="F3" s="50"/>
       <c r="G3" s="53"/>
       <c r="H3" s="54"/>
-      <c r="I3" s="71" t="s">
+      <c r="I3" s="77" t="s">
         <v>78</v>
       </c>
-      <c r="J3" s="72"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="78" t="s">
-        <v>86</v>
-      </c>
-      <c r="M3" s="79"/>
-      <c r="N3" s="80"/>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1">
+      <c r="J3" s="78"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="80" t="s">
+        <v>84</v>
+      </c>
+      <c r="M3" s="81"/>
+      <c r="N3" s="82"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50"/>
       <c r="B4" s="51"/>
       <c r="C4" s="52"/>
@@ -2428,19 +2494,19 @@
       <c r="F4" s="50"/>
       <c r="G4" s="53"/>
       <c r="H4" s="54"/>
-      <c r="I4" s="68" t="s">
-        <v>83</v>
-      </c>
-      <c r="J4" s="69"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="82">
+      <c r="I4" s="74" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="75"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="68">
         <v>38539</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="86"/>
-    </row>
-    <row r="5" spans="1:15" ht="50.25" customHeight="1">
-      <c r="A5" s="65" t="s">
+      <c r="M4" s="69"/>
+      <c r="N4" s="70"/>
+    </row>
+    <row r="5" spans="1:15" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="71" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="49" t="s">
@@ -2464,27 +2530,27 @@
       <c r="H5" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="J5" s="62" t="s">
-        <v>84</v>
-      </c>
-      <c r="K5" s="83" t="s">
-        <v>79</v>
-      </c>
-      <c r="L5" s="88" t="s">
-        <v>84</v>
-      </c>
-      <c r="M5" s="89" t="s">
-        <v>84</v>
-      </c>
-      <c r="N5" s="90" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="42.75" customHeight="1">
-      <c r="A6" s="66"/>
+      <c r="I5" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="L5" s="84" t="s">
+        <v>83</v>
+      </c>
+      <c r="M5" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="N5" s="86" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="72"/>
       <c r="B6" s="38" t="s">
         <v>60</v>
       </c>
@@ -2506,27 +2572,27 @@
       <c r="H6" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="57" t="s">
-        <v>79</v>
-      </c>
-      <c r="J6" s="64" t="s">
-        <v>84</v>
+      <c r="I6" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>83</v>
       </c>
       <c r="K6" s="84" t="s">
-        <v>79</v>
-      </c>
-      <c r="L6" s="91" t="s">
-        <v>84</v>
-      </c>
-      <c r="M6" s="87" t="s">
-        <v>84</v>
-      </c>
-      <c r="N6" s="92" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="43.5" customHeight="1">
-      <c r="A7" s="66"/>
+        <v>85</v>
+      </c>
+      <c r="L6" s="87" t="s">
+        <v>83</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="N6" s="88" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="72"/>
       <c r="B7" s="38"/>
       <c r="C7" s="29">
         <v>3</v>
@@ -2546,27 +2612,27 @@
       <c r="H7" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="63" t="s">
-        <v>85</v>
-      </c>
-      <c r="J7" s="58" t="s">
-        <v>84</v>
-      </c>
-      <c r="K7" s="85" t="s">
-        <v>85</v>
-      </c>
-      <c r="L7" s="91" t="s">
-        <v>84</v>
-      </c>
-      <c r="M7" s="87" t="s">
-        <v>84</v>
-      </c>
-      <c r="N7" s="92" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="50.25" customHeight="1">
-      <c r="A8" s="66"/>
+      <c r="I7" s="89" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" s="89" t="s">
+        <v>86</v>
+      </c>
+      <c r="L7" s="87" t="s">
+        <v>83</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="N7" s="88" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="72"/>
       <c r="B8" s="38"/>
       <c r="C8" s="29">
         <v>4</v>
@@ -2574,57 +2640,57 @@
       <c r="D8" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="101">
+      <c r="E8" s="60">
         <v>0</v>
       </c>
-      <c r="F8" s="102" t="s">
+      <c r="F8" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="103" t="s">
+      <c r="G8" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="H8" s="104" t="s">
+      <c r="H8" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="I8" s="105" t="s">
+      <c r="I8" s="89" t="s">
+        <v>86</v>
+      </c>
+      <c r="J8" s="90" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" s="89" t="s">
+        <v>86</v>
+      </c>
+      <c r="L8" s="91" t="s">
         <v>85</v>
       </c>
-      <c r="J8" s="106" t="s">
-        <v>84</v>
-      </c>
-      <c r="K8" s="107" t="s">
+      <c r="M8" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="L8" s="98" t="s">
-        <v>87</v>
-      </c>
-      <c r="M8" s="99" t="s">
-        <v>87</v>
-      </c>
-      <c r="N8" s="100" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="50.25" customHeight="1" thickBot="1">
-      <c r="A9" s="67"/>
+      <c r="N8" s="92" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="73"/>
       <c r="B9" s="38"/>
-      <c r="C9" s="113">
+      <c r="C9" s="65">
         <v>41278</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="27"/>
       <c r="F9" s="23"/>
       <c r="G9" s="27"/>
-      <c r="H9" s="111"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="87"/>
-      <c r="M9" s="87"/>
-      <c r="N9" s="112"/>
-    </row>
-    <row r="10" spans="1:15" s="7" customFormat="1" ht="58.5" customHeight="1">
-      <c r="A10" s="65" t="s">
+      <c r="H9" s="64"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="23"/>
+    </row>
+    <row r="10" spans="1:15" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="71" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="49" t="s">
@@ -2645,24 +2711,24 @@
       <c r="G10" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="104" t="s">
+      <c r="H10" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="61"/>
+      <c r="I10" s="56"/>
       <c r="J10" s="33"/>
-      <c r="K10" s="96"/>
-      <c r="L10" s="108" t="s">
-        <v>87</v>
-      </c>
-      <c r="M10" s="109" t="s">
-        <v>87</v>
-      </c>
-      <c r="N10" s="110" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="58.5" customHeight="1">
-      <c r="A11" s="66"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="M10" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="N10" s="83" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="72"/>
       <c r="B11" s="38" t="s">
         <v>61</v>
       </c>
@@ -2684,21 +2750,21 @@
       <c r="H11" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="57"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="84"/>
-      <c r="L11" s="91" t="s">
-        <v>87</v>
-      </c>
-      <c r="M11" s="87" t="s">
-        <v>87</v>
-      </c>
-      <c r="N11" s="92" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="63" customHeight="1">
-      <c r="A12" s="66"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="93"/>
+      <c r="L11" s="87" t="s">
+        <v>85</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="N11" s="88" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="72"/>
       <c r="B12" s="38"/>
       <c r="C12" s="35">
         <v>3</v>
@@ -2718,15 +2784,15 @@
       <c r="H12" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="57"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="84"/>
-      <c r="L12" s="91"/>
-      <c r="M12" s="87"/>
-      <c r="N12" s="92"/>
-    </row>
-    <row r="13" spans="1:15" ht="45" customHeight="1" thickBot="1">
-      <c r="A13" s="67"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="93"/>
+      <c r="L12" s="87"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="88"/>
+    </row>
+    <row r="13" spans="1:15" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="73"/>
       <c r="B13" s="39"/>
       <c r="C13" s="28">
         <v>4</v>
@@ -2746,14 +2812,14 @@
       <c r="H13" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="59"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="97"/>
-      <c r="L13" s="93"/>
-      <c r="M13" s="94"/>
-      <c r="N13" s="95"/>
-    </row>
-    <row r="17" spans="4:8">
+      <c r="I13" s="94"/>
+      <c r="J13" s="95"/>
+      <c r="K13" s="96"/>
+      <c r="L13" s="94"/>
+      <c r="M13" s="95"/>
+      <c r="N13" s="97"/>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17" s="48" t="s">
         <v>74</v>
       </c>
@@ -2763,8 +2829,6 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="L4:N4"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="I4:K4"/>
@@ -2772,6 +2836,8 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="L4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Analyzed test results for B.1.0 / MID Innovator.
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="87">
   <si>
     <t>Documentation</t>
   </si>
@@ -1584,11 +1584,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1598,87 +1679,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2411,8 +2411,8 @@
   </sheetPr>
   <dimension ref="A2:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2427,18 +2427,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="66" t="s">
+      <c r="B2" s="91"/>
+      <c r="C2" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="67"/>
-      <c r="E2" s="66" t="s">
+      <c r="D2" s="91"/>
+      <c r="E2" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="67"/>
+      <c r="F2" s="91"/>
       <c r="G2" s="24" t="s">
         <v>36</v>
       </c>
@@ -2474,16 +2474,16 @@
       <c r="F3" s="50"/>
       <c r="G3" s="53"/>
       <c r="H3" s="54"/>
-      <c r="I3" s="77" t="s">
+      <c r="I3" s="87" t="s">
         <v>78</v>
       </c>
-      <c r="J3" s="78"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="80" t="s">
+      <c r="J3" s="88"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="92" t="s">
         <v>84</v>
       </c>
-      <c r="M3" s="81"/>
-      <c r="N3" s="82"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="94"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50"/>
@@ -2494,19 +2494,19 @@
       <c r="F4" s="50"/>
       <c r="G4" s="53"/>
       <c r="H4" s="54"/>
-      <c r="I4" s="74" t="s">
+      <c r="I4" s="84" t="s">
         <v>82</v>
       </c>
-      <c r="J4" s="75"/>
-      <c r="K4" s="76"/>
-      <c r="L4" s="68">
+      <c r="J4" s="85"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="95">
         <v>38539</v>
       </c>
-      <c r="M4" s="69"/>
-      <c r="N4" s="70"/>
+      <c r="M4" s="96"/>
+      <c r="N4" s="97"/>
     </row>
     <row r="5" spans="1:15" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="81" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="49" t="s">
@@ -2530,27 +2530,27 @@
       <c r="H5" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="84" t="s">
+      <c r="I5" s="67" t="s">
         <v>85</v>
       </c>
       <c r="J5" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="K5" s="84" t="s">
+      <c r="K5" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="84" t="s">
+      <c r="L5" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="M5" s="85" t="s">
+      <c r="M5" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="N5" s="86" t="s">
+      <c r="N5" s="69" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="72"/>
+      <c r="A6" s="82"/>
       <c r="B6" s="38" t="s">
         <v>60</v>
       </c>
@@ -2572,27 +2572,27 @@
       <c r="H6" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="84" t="s">
+      <c r="I6" s="67" t="s">
         <v>85</v>
       </c>
       <c r="J6" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="K6" s="84" t="s">
+      <c r="K6" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="L6" s="87" t="s">
+      <c r="L6" s="70" t="s">
         <v>83</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="N6" s="88" t="s">
+      <c r="N6" s="71" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="72"/>
+      <c r="A7" s="82"/>
       <c r="B7" s="38"/>
       <c r="C7" s="29">
         <v>3</v>
@@ -2612,27 +2612,27 @@
       <c r="H7" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="89" t="s">
+      <c r="I7" s="72" t="s">
         <v>86</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="K7" s="89" t="s">
+      <c r="K7" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="L7" s="87" t="s">
+      <c r="L7" s="70" t="s">
         <v>83</v>
       </c>
       <c r="M7" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="N7" s="88" t="s">
+      <c r="N7" s="71" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="72"/>
+      <c r="A8" s="82"/>
       <c r="B8" s="38"/>
       <c r="C8" s="29">
         <v>4</v>
@@ -2652,27 +2652,27 @@
       <c r="H8" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="I8" s="89" t="s">
+      <c r="I8" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="J8" s="90" t="s">
+      <c r="J8" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="K8" s="89" t="s">
+      <c r="K8" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="L8" s="91" t="s">
+      <c r="L8" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="M8" s="90" t="s">
+      <c r="M8" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="N8" s="92" t="s">
+      <c r="N8" s="75" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="73"/>
+      <c r="A9" s="83"/>
       <c r="B9" s="38"/>
       <c r="C9" s="65">
         <v>41278</v>
@@ -2690,7 +2690,7 @@
       <c r="N9" s="23"/>
     </row>
     <row r="10" spans="1:15" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="71" t="s">
+      <c r="A10" s="81" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="49" t="s">
@@ -2714,8 +2714,12 @@
       <c r="H10" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="56"/>
-      <c r="J10" s="33"/>
+      <c r="I10" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="J10" s="33" t="s">
+        <v>85</v>
+      </c>
       <c r="K10" s="59"/>
       <c r="L10" s="56" t="s">
         <v>85</v>
@@ -2723,12 +2727,12 @@
       <c r="M10" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="N10" s="83" t="s">
+      <c r="N10" s="66" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="72"/>
+      <c r="A11" s="82"/>
       <c r="B11" s="38" t="s">
         <v>61</v>
       </c>
@@ -2750,21 +2754,21 @@
       <c r="H11" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="87"/>
+      <c r="I11" s="70"/>
       <c r="J11" s="8"/>
-      <c r="K11" s="93"/>
-      <c r="L11" s="87" t="s">
+      <c r="K11" s="76"/>
+      <c r="L11" s="70" t="s">
         <v>85</v>
       </c>
       <c r="M11" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="N11" s="88" t="s">
+      <c r="N11" s="71" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="72"/>
+      <c r="A12" s="82"/>
       <c r="B12" s="38"/>
       <c r="C12" s="35">
         <v>3</v>
@@ -2784,15 +2788,15 @@
       <c r="H12" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="87"/>
+      <c r="I12" s="70"/>
       <c r="J12" s="8"/>
-      <c r="K12" s="93"/>
-      <c r="L12" s="87"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="70"/>
       <c r="M12" s="8"/>
-      <c r="N12" s="88"/>
+      <c r="N12" s="71"/>
     </row>
     <row r="13" spans="1:15" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="73"/>
+      <c r="A13" s="83"/>
       <c r="B13" s="39"/>
       <c r="C13" s="28">
         <v>4</v>
@@ -2812,12 +2816,12 @@
       <c r="H13" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="94"/>
-      <c r="J13" s="95"/>
-      <c r="K13" s="96"/>
-      <c r="L13" s="94"/>
-      <c r="M13" s="95"/>
-      <c r="N13" s="97"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="79"/>
+      <c r="L13" s="77"/>
+      <c r="M13" s="78"/>
+      <c r="N13" s="80"/>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17" s="48" t="s">
@@ -2829,6 +2833,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="L4:N4"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="I4:K4"/>
@@ -2836,8 +2842,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="L4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>

</xml_diff>